<commit_message>
implementation of phase completion status
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata_localstg.xlsx
+++ b/src/main/java/dataRepository/logindata_localstg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -28,22 +28,67 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">exu156@mailinator.com</t>
+    <t xml:space="preserve">auttestt_41@mailinator.com</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">exu157@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exu158@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exu159@mailinator.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exu160@mailinator.com</t>
+    <t xml:space="preserve">auttestt_42@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_43@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_44@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_45@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_46@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_47@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_48@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_49@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_50@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_51@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_52@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_53@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_54@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_55@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_56@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_57@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_58@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_59@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttestt_60@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -151,20 +196,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="27.530612244898" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="8.77551020408163" collapsed="true"/>
-    <col min="3" max="7" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="25.1071428571429" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="18.4948979591837" collapsed="true"/>
-    <col min="10" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="25.3775510204082" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="8.23469387755102" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="23.0816326530612" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="17.0102040816327" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="8.23469387755102" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,6 +218,118 @@
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed chrome driver from server
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata_localstg.xlsx
+++ b/src/main/java/dataRepository/logindata_localstg.xlsx
@@ -147,10 +147,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2602040816327"/>
+    <col min="1" max="1" hidden="false" style="0" width="36.1785714285714" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.530612244898" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="14.5816326530612" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="10.2602040816327" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -159,14 +159,6 @@
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>